<commit_message>
added piano class to admin page
</commit_message>
<xml_diff>
--- a/resources/GPS_code_copy.xlsx
+++ b/resources/GPS_code_copy.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="190">
   <si>
     <r>
       <t xml:space="preserve">from </t>
@@ -1443,12 +1443,6 @@
     </r>
   </si>
   <si>
-    <t>path:GreatPSproj\accpountapp</t>
-  </si>
-  <si>
-    <t>urlsk.py</t>
-  </si>
-  <si>
     <t>"""Projectproj URL Configuration</t>
   </si>
   <si>
@@ -1679,13 +1673,1957 @@
   </si>
   <si>
     <t>]</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">from </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">django </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">import </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>forms</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">from </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">django.contrib.auth.forms </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">import </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>UserCreationForm</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">from </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">accountapp.models </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">import </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>User</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">class </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>CustomUserCreationForm(UserCreationForm):</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">class </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>Meta(UserCreationForm.Meta):</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">         model = User</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">         fields = UserCreationForm.Meta.fields + ( </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'email'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'username'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>forms.py</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">from </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">django.apps </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">import </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>AppConfig</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">class </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>AccountappConfig(AppConfig):</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    name = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'accountapp'</t>
+    </r>
+  </si>
+  <si>
+    <t>app.py</t>
+  </si>
+  <si>
+    <t>accounts\models.py</t>
+  </si>
+  <si>
+    <t>accounts\login.html</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">&lt;!DOCTYPE </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>html</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">html </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>lang=</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>"en"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>head</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">meta </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>charset=</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>"UTF-8"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>title</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;Login&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>title</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>head</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>body</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">form </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>action=</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">"" </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>method=</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>"POSt"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">      {%csrf_token %}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      {{form.as_p}}</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">      &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>button</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;LogIn&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>button</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>form</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>body</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>html</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>title</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;Registration/Login Form&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>title</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">    {%csrf_token %}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    {{form.as_p}}</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>button</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;LogIn&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>button</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>register.html</t>
+  </si>
+  <si>
+    <t>settings.py</t>
+  </si>
+  <si>
+    <t>Django settings for GreatPSproj project.</t>
+  </si>
+  <si>
+    <t>Generated by 'django-admin startproject' using Django 1.11.3.</t>
+  </si>
+  <si>
+    <t>For more information on this file, see</t>
+  </si>
+  <si>
+    <t>https://docs.djangoproject.com/en/1.11/topics/settings/</t>
+  </si>
+  <si>
+    <t>For the full list of settings and their values, see</t>
+  </si>
+  <si>
+    <t>https://docs.djangoproject.com/en/1.11/ref/settings/</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">import </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>os</t>
+    </r>
+  </si>
+  <si>
+    <t># Build paths inside the project like this: os.path.join(BASE_DIR, ...)</t>
+  </si>
+  <si>
+    <t>BASE_DIR = os.path.dirname(os.path.dirname(os.path.abspath(__file__)))</t>
+  </si>
+  <si>
+    <t># Quick-start development settings - unsuitable for production</t>
+  </si>
+  <si>
+    <t># See https://docs.djangoproject.com/en/1.11/howto/deployment/checklist/</t>
+  </si>
+  <si>
+    <t># SECURITY WARNING: keep the secret key used in production secret!</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SECRET_KEY = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'k1q7flod3e%vnzpurexz74)f+)rn*+lu)vi2w28w5bz#_i)9xj'</t>
+    </r>
+  </si>
+  <si>
+    <t># SECURITY WARNING: don't run with debug turned on in production!</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">DEBUG = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>True</t>
+    </r>
+  </si>
+  <si>
+    <t>ALLOWED_HOSTS = []</t>
+  </si>
+  <si>
+    <t># Application definition</t>
+  </si>
+  <si>
+    <t>INSTALLED_APPS = [</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'django.contrib.admin'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'django.contrib.auth'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'django.contrib.contenttypes'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'django.contrib.sessions'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'django.contrib.messages'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'django.contrib.staticfiles'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'GreatPSapp'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'accountapp'</t>
+    </r>
+  </si>
+  <si>
+    <t>MIDDLEWARE = [</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'django.middleware.security.SecurityMiddleware'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'django.contrib.sessions.middleware.SessionMiddleware'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'django.middleware.common.CommonMiddleware'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'django.middleware.csrf.CsrfViewMiddleware'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'django.contrib.auth.middleware.AuthenticationMiddleware'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'django.contrib.messages.middleware.MessageMiddleware'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'django.middleware.clickjacking.XFrameOptionsMiddleware'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ROOT_URLCONF = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'GreatPSproj.urls'</t>
+    </r>
+  </si>
+  <si>
+    <t>TEMPLATES = [</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    {</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'BACKEND'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'django.template.backends.django.DjangoTemplates'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'DIRS'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>: [],</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'APP_DIRS'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>True</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'OPTIONS'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>: {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">            </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'context_processors'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>: [</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'django.template.context_processors.debug'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'django.template.context_processors.request'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'django.contrib.auth.context_processors.auth'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'django.contrib.messages.context_processors.messages'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">            ],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    },</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">WSGI_APPLICATION = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'GreatPSproj.wsgi.application'</t>
+    </r>
+  </si>
+  <si>
+    <t># Database</t>
+  </si>
+  <si>
+    <t># https://docs.djangoproject.com/en/1.11/ref/settings/#databases</t>
+  </si>
+  <si>
+    <t>DATABASES = {</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'default'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>: {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'ENGINE'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'django.db.backends.sqlite3'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'NAME'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">: os.path.join(BASE_DIR, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'db.sqlite3'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>),</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">    }</t>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">AUTH_USER_MODEL = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'accountapp.User'</t>
+    </r>
+  </si>
+  <si>
+    <t># Password validation</t>
+  </si>
+  <si>
+    <t># https://docs.djangoproject.com/en/1.11/ref/settings/#auth-password-validators</t>
+  </si>
+  <si>
+    <t>AUTH_PASSWORD_VALIDATORS = [</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'NAME'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'django.contrib.auth.password_validation.UserAttributeSimilarityValidator'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'NAME'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'django.contrib.auth.password_validation.MinimumLengthValidator'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'NAME'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'django.contrib.auth.password_validation.CommonPasswordValidator'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'NAME'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'django.contrib.auth.password_validation.NumericPasswordValidator'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <t># Internationalization</t>
+  </si>
+  <si>
+    <t># https://docs.djangoproject.com/en/1.11/topics/i18n/</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">LANGUAGE_CODE = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'en-us'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">TIME_ZONE = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'UTC'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">USE_I18N = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>True</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">USE_L10N = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>True</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">USE_TZ = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>True</t>
+    </r>
+  </si>
+  <si>
+    <t># Static files (CSS, JavaScript, Images)</t>
+  </si>
+  <si>
+    <t># https://docs.djangoproject.com/en/1.11/howto/static-files/</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">STATIC_URL = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'/static/'</t>
+    </r>
+  </si>
+  <si>
+    <t>GreatPSproj\GreatPSproj\accpountapp</t>
+  </si>
+  <si>
+    <t>urls.py</t>
+  </si>
+  <si>
+    <t>GreatPSproj\GreatPSproj\accpountapp\</t>
+  </si>
+  <si>
+    <t>GreatPSproj\GreatPSproj\accpountapp\templates</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1744,8 +3682,22 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9.6"/>
+      <color rgb="FF0000FF"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9.6"/>
+      <color rgb="FF008000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1755,6 +3707,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEFEFEF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1786,7 +3744,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1805,6 +3763,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2121,410 +4082,1039 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E58"/>
+  <dimension ref="A1:J124"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1:C1048576"/>
+      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="9" width="44.5546875" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="10" width="44.5546875" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>55</v>
+        <v>186</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>186</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>55</v>
+        <v>186</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="B2" s="1" t="s">
+        <v>109</v>
+      </c>
       <c r="D2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="26.4" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="B3" s="7" t="s">
+        <v>68</v>
+      </c>
       <c r="D3" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="26.4" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="B4" s="6" t="s">
+        <v>110</v>
+      </c>
       <c r="D4" s="3" t="s">
         <v>19</v>
       </c>
       <c r="E4" s="4"/>
-    </row>
-    <row r="5" spans="1:5" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="F4" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
       <c r="D5" s="3" t="s">
         <v>20</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="39.6" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
+      <c r="B6" s="6" t="s">
+        <v>111</v>
+      </c>
       <c r="D6" s="4"/>
       <c r="E6" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="26.4" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="H6" s="4"/>
+      <c r="I6" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
       <c r="D7" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+      <c r="F7" s="4"/>
+      <c r="G7" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="H7" s="4"/>
+      <c r="I7" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="39" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
+      <c r="B8" s="6" t="s">
+        <v>112</v>
+      </c>
       <c r="D8" s="4"/>
       <c r="E8" s="6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="26.4" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="B9" s="6" t="s">
+        <v>113</v>
+      </c>
       <c r="D9" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="26.4" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+      <c r="F9" s="4"/>
+      <c r="H9" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>3</v>
       </c>
+      <c r="B10" s="4"/>
       <c r="D10" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="26.4" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>4</v>
       </c>
+      <c r="B11" s="6" t="s">
+        <v>114</v>
+      </c>
       <c r="D11" s="3" t="s">
         <v>24</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="26.4" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="38.4" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>5</v>
       </c>
+      <c r="B12" s="6" t="s">
+        <v>115</v>
+      </c>
       <c r="D12" s="3" t="s">
         <v>25</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="39.6" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>6</v>
       </c>
+      <c r="B13" s="6" t="s">
+        <v>68</v>
+      </c>
       <c r="D13" s="4"/>
       <c r="E13" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+      <c r="H13" s="4"/>
+      <c r="I13" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="39.6" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>7</v>
       </c>
+      <c r="B15" s="3" t="s">
+        <v>116</v>
+      </c>
       <c r="D15" s="3" t="s">
         <v>26</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="26.4" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+    </row>
+    <row r="16" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>8</v>
       </c>
+      <c r="B17" s="6" t="s">
+        <v>117</v>
+      </c>
       <c r="D17" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="38.4" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+      <c r="H17" s="4"/>
+      <c r="I17" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="38.4" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
+      <c r="B18" s="5" t="s">
+        <v>118</v>
+      </c>
       <c r="D18" s="5" t="s">
         <v>28</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>9</v>
       </c>
+      <c r="B19" s="4"/>
       <c r="D19" s="5" t="s">
         <v>29</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="38.4" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="38.4" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>10</v>
       </c>
+      <c r="B20" s="4"/>
       <c r="D20" s="5" t="s">
         <v>30</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="B21" s="6" t="s">
+        <v>119</v>
+      </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
     </row>
-    <row r="22" spans="1:5" ht="25.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>12</v>
       </c>
+      <c r="B22" s="6" t="s">
+        <v>120</v>
+      </c>
       <c r="D22" s="5" t="s">
         <v>31</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="25.8" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="25.8" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>13</v>
       </c>
+      <c r="B23" s="4"/>
       <c r="D23" s="5" t="s">
         <v>32</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="26.4" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>14</v>
       </c>
+      <c r="B24" s="6" t="s">
+        <v>121</v>
+      </c>
       <c r="D24" s="5" t="s">
         <v>33</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="39" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="B25" s="5" t="s">
+        <v>122</v>
+      </c>
       <c r="D25" s="6" t="s">
         <v>34</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B26" s="4"/>
       <c r="D26" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="B27" s="6" t="s">
+        <v>123</v>
+      </c>
       <c r="D27" s="4"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B28" s="5" t="s">
+        <v>124</v>
+      </c>
       <c r="D28" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="B29" s="4"/>
       <c r="D29" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B30" s="5" t="s">
+        <v>125</v>
+      </c>
       <c r="D30" s="4"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B31" s="4"/>
       <c r="D31" s="4"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B32" s="4"/>
       <c r="D32" s="4"/>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B33" s="6" t="s">
+        <v>126</v>
+      </c>
       <c r="D33" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B34" s="4"/>
       <c r="D34" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B35" s="5" t="s">
+        <v>127</v>
+      </c>
       <c r="D35" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B36" s="5" t="s">
+        <v>128</v>
+      </c>
       <c r="D36" s="4"/>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B37" s="5" t="s">
+        <v>129</v>
+      </c>
       <c r="D37" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B38" s="5" t="s">
+        <v>130</v>
+      </c>
       <c r="D38" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B39" s="5" t="s">
+        <v>131</v>
+      </c>
       <c r="D39" s="4"/>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B40" s="5" t="s">
+        <v>132</v>
+      </c>
       <c r="D40" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="41" spans="4:4" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:4" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="B41" s="5" t="s">
+        <v>133</v>
+      </c>
       <c r="D41" s="6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="42" spans="4:4" ht="25.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:4" ht="25.8" x14ac:dyDescent="0.3">
+      <c r="B42" s="5" t="s">
+        <v>134</v>
+      </c>
       <c r="D42" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B43" s="5" t="s">
+        <v>135</v>
+      </c>
       <c r="D43" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="44" spans="4:4" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:4" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="B44" s="5" t="s">
+        <v>75</v>
+      </c>
       <c r="D44" s="6" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B45" s="4"/>
       <c r="D45" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B46" s="5" t="s">
+        <v>136</v>
+      </c>
       <c r="D46" s="4"/>
     </row>
-    <row r="47" spans="4:4" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:4" ht="39" x14ac:dyDescent="0.3">
+      <c r="B47" s="5" t="s">
+        <v>137</v>
+      </c>
       <c r="D47" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="4:4" ht="39" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:4" ht="39" x14ac:dyDescent="0.3">
+      <c r="B48" s="5" t="s">
+        <v>138</v>
+      </c>
       <c r="D48" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:4" ht="39" x14ac:dyDescent="0.3">
+      <c r="B49" s="5" t="s">
+        <v>139</v>
+      </c>
       <c r="D49" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:4" ht="39" x14ac:dyDescent="0.3">
+      <c r="B50" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="D50" s="4"/>
     </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:4" ht="39" x14ac:dyDescent="0.3">
+      <c r="B51" s="5" t="s">
+        <v>141</v>
+      </c>
       <c r="D51" s="4"/>
     </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:4" ht="39" x14ac:dyDescent="0.3">
+      <c r="B52" s="5" t="s">
+        <v>142</v>
+      </c>
       <c r="D52" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="53" spans="4:4" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:4" ht="39" x14ac:dyDescent="0.3">
+      <c r="B53" s="5" t="s">
+        <v>143</v>
+      </c>
       <c r="D53" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B54" s="5" t="s">
+        <v>75</v>
+      </c>
       <c r="D54" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="55" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B55" s="4"/>
       <c r="D55" s="6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="56" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B56" s="5" t="s">
+        <v>144</v>
+      </c>
       <c r="D56" s="4"/>
     </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B57" s="4"/>
       <c r="D57" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="58" spans="4:4" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:4" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="B58" s="5" t="s">
+        <v>145</v>
+      </c>
       <c r="D58" s="5" t="s">
         <v>54</v>
       </c>
     </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B59" s="5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="B60" s="5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B61" s="5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B62" s="5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B63" s="5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B64" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" ht="39" x14ac:dyDescent="0.3">
+      <c r="B65" s="5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" ht="39" x14ac:dyDescent="0.3">
+      <c r="B66" s="5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2" ht="39" x14ac:dyDescent="0.3">
+      <c r="B67" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2" ht="39" x14ac:dyDescent="0.3">
+      <c r="B68" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B69" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B70" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B71" s="5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B72" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B73" s="4"/>
+    </row>
+    <row r="74" spans="2:2" ht="25.8" x14ac:dyDescent="0.3">
+      <c r="B74" s="5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B75" s="4"/>
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B76" s="4"/>
+    </row>
+    <row r="77" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B77" s="6" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="78" spans="2:2" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="B78" s="6" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="79" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B79" s="4"/>
+    </row>
+    <row r="80" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B80" s="5" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B81" s="5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="B82" s="5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="83" spans="2:2" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="B83" s="5" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B84" s="5" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B85" s="5" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B86" s="4"/>
+    </row>
+    <row r="87" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B87" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B88" s="6" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="89" spans="2:2" ht="52.8" x14ac:dyDescent="0.3">
+      <c r="B89" s="6" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="90" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B90" s="4"/>
+    </row>
+    <row r="91" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B91" s="5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="92" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B92" s="5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="93" spans="2:2" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="B93" s="5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="94" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B94" s="5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="95" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B95" s="5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="96" spans="2:2" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="B96" s="5" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B97" s="5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="98" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B98" s="5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="99" spans="2:2" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="B99" s="5" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="100" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B100" s="5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="101" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B101" s="5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="102" spans="2:2" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="B102" s="5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="103" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B103" s="5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="104" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B104" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="105" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B105" s="4"/>
+    </row>
+    <row r="106" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B106" s="4"/>
+    </row>
+    <row r="107" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B107" s="6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="108" spans="2:2" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="B108" s="6" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="109" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B109" s="4"/>
+    </row>
+    <row r="110" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B110" s="5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="111" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B111" s="4"/>
+    </row>
+    <row r="112" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B112" s="5" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="113" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B113" s="4"/>
+    </row>
+    <row r="114" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B114" s="5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="115" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B115" s="4"/>
+    </row>
+    <row r="116" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B116" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="117" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B117" s="4"/>
+    </row>
+    <row r="118" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B118" s="5" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="119" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B119" s="4"/>
+    </row>
+    <row r="120" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B120" s="4"/>
+    </row>
+    <row r="121" spans="2:2" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="B121" s="6" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="122" spans="2:2" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="B122" s="6" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="123" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B123" s="4"/>
+    </row>
+    <row r="124" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B124" s="5" t="s">
+        <v>185</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>